<commit_message>
"Added code for Inv Loc to Loc- serial track item"
</commit_message>
<xml_diff>
--- a/templates/LocationToLocation.xlsx
+++ b/templates/LocationToLocation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\provar\rsqasampleproj\rsqasampleproj\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31BF1862-5A8F-443B-839B-10C4787DFEAC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADA8EB60-665C-4675-83DE-9DF5C995C2AD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{AAD229B4-EC82-43D3-8B6F-DC67705348E6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{AAD229B4-EC82-43D3-8B6F-DC67705348E6}"/>
   </bookViews>
   <sheets>
     <sheet name="LotTrack_NoTrack" sheetId="1" r:id="rId1"/>
@@ -95,9 +95,6 @@
     <t>Test Provar-Serial</t>
   </si>
   <si>
-    <t>Provar-118,Provar-119</t>
-  </si>
-  <si>
     <t>Lot No</t>
   </si>
   <si>
@@ -258,6 +255,9 @@
   </si>
   <si>
     <t>P-5V1I</t>
+  </si>
+  <si>
+    <t>Provar-120,Provar-121</t>
   </si>
 </sst>
 </file>
@@ -626,7 +626,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BB0B39B-4FD7-48BF-9EEB-2258D69FB641}">
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
@@ -656,7 +656,7 @@
         <v>12</v>
       </c>
       <c r="E1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F1" t="s">
         <v>13</v>
@@ -679,31 +679,31 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D2">
         <v>777</v>
       </c>
       <c r="E2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F2" t="s">
         <v>15</v>
       </c>
       <c r="G2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I2">
         <v>15</v>
       </c>
       <c r="J2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -711,31 +711,31 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D3">
         <v>777</v>
       </c>
       <c r="E3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" t="s">
         <v>25</v>
       </c>
-      <c r="F3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" t="s">
-        <v>26</v>
-      </c>
       <c r="H3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I3">
         <v>5</v>
       </c>
       <c r="J3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
@@ -743,31 +743,31 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D4">
         <v>777</v>
       </c>
       <c r="E4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F4" t="s">
         <v>15</v>
       </c>
       <c r="G4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" t="s">
         <v>28</v>
-      </c>
-      <c r="H4" t="s">
-        <v>29</v>
       </c>
       <c r="I4">
         <v>6</v>
       </c>
       <c r="J4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
@@ -775,31 +775,31 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D5">
         <v>777</v>
       </c>
       <c r="E5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F5" t="s">
         <v>15</v>
       </c>
       <c r="G5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H5" t="s">
         <v>31</v>
-      </c>
-      <c r="H5" t="s">
-        <v>32</v>
       </c>
       <c r="I5">
         <v>8</v>
       </c>
       <c r="J5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
@@ -807,31 +807,31 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D6">
         <v>777</v>
       </c>
       <c r="E6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F6" t="s">
         <v>15</v>
       </c>
       <c r="G6" t="s">
+        <v>38</v>
+      </c>
+      <c r="H6" t="s">
         <v>39</v>
-      </c>
-      <c r="H6" t="s">
-        <v>40</v>
       </c>
       <c r="I6">
         <v>75</v>
       </c>
       <c r="J6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
@@ -839,31 +839,31 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F7" t="s">
         <v>15</v>
       </c>
       <c r="G7" t="s">
+        <v>38</v>
+      </c>
+      <c r="H7" t="s">
         <v>39</v>
-      </c>
-      <c r="H7" t="s">
-        <v>40</v>
       </c>
       <c r="I7">
         <v>5</v>
       </c>
       <c r="J7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
@@ -871,31 +871,31 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F8" t="s">
         <v>15</v>
       </c>
       <c r="G8" t="s">
+        <v>30</v>
+      </c>
+      <c r="H8" t="s">
         <v>31</v>
-      </c>
-      <c r="H8" t="s">
-        <v>32</v>
       </c>
       <c r="I8">
         <v>4.5490000000000004</v>
       </c>
       <c r="J8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
@@ -903,31 +903,31 @@
         <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" t="s">
+        <v>20</v>
+      </c>
+      <c r="H9" t="s">
         <v>29</v>
-      </c>
-      <c r="E9" t="s">
-        <v>25</v>
-      </c>
-      <c r="F9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G9" t="s">
-        <v>21</v>
-      </c>
-      <c r="H9" t="s">
-        <v>30</v>
       </c>
       <c r="I9">
         <v>3.3544999999999998</v>
       </c>
       <c r="J9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
@@ -935,31 +935,31 @@
         <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F10">
         <v>1003</v>
       </c>
       <c r="G10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I10">
         <v>11.656478999999999</v>
       </c>
       <c r="J10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
@@ -967,31 +967,31 @@
         <v>4</v>
       </c>
       <c r="B11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D11" t="s">
+        <v>41</v>
+      </c>
+      <c r="E11" t="s">
+        <v>44</v>
+      </c>
+      <c r="F11" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" t="s">
         <v>42</v>
       </c>
-      <c r="E11" t="s">
-        <v>45</v>
-      </c>
-      <c r="F11" t="s">
-        <v>15</v>
-      </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
         <v>43</v>
-      </c>
-      <c r="H11" t="s">
-        <v>44</v>
       </c>
       <c r="I11">
         <v>2.6558999999999999</v>
       </c>
       <c r="J11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
@@ -999,63 +999,63 @@
         <v>4</v>
       </c>
       <c r="B12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C12" t="s">
         <v>16</v>
       </c>
       <c r="D12" t="s">
+        <v>45</v>
+      </c>
+      <c r="E12" t="s">
         <v>46</v>
-      </c>
-      <c r="E12" t="s">
-        <v>47</v>
       </c>
       <c r="F12">
         <v>1005</v>
       </c>
       <c r="G12" t="s">
+        <v>38</v>
+      </c>
+      <c r="H12" t="s">
         <v>39</v>
-      </c>
-      <c r="H12" t="s">
-        <v>40</v>
       </c>
       <c r="I12">
         <v>30.545999999999999</v>
       </c>
       <c r="J12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D13">
         <v>1</v>
       </c>
       <c r="E13" t="s">
+        <v>36</v>
+      </c>
+      <c r="F13" t="s">
+        <v>15</v>
+      </c>
+      <c r="G13" t="s">
+        <v>23</v>
+      </c>
+      <c r="H13" t="s">
         <v>37</v>
-      </c>
-      <c r="F13" t="s">
-        <v>15</v>
-      </c>
-      <c r="G13" t="s">
-        <v>24</v>
-      </c>
-      <c r="H13" t="s">
-        <v>38</v>
       </c>
       <c r="I13">
         <v>1</v>
       </c>
       <c r="J13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
@@ -1069,19 +1069,19 @@
         <v>14</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F14" t="s">
         <v>15</v>
       </c>
       <c r="G14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I14">
         <v>4.6546000000000003</v>
       </c>
       <c r="J14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
@@ -1092,22 +1092,22 @@
         <v>10</v>
       </c>
       <c r="C15" t="s">
+        <v>61</v>
+      </c>
+      <c r="D15" t="s">
         <v>62</v>
       </c>
-      <c r="D15" t="s">
-        <v>63</v>
-      </c>
       <c r="F15" t="s">
         <v>15</v>
       </c>
       <c r="G15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I15">
         <v>2</v>
       </c>
       <c r="J15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
@@ -1133,7 +1133,7 @@
         <v>1.2465999999999999</v>
       </c>
       <c r="J16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
@@ -1147,19 +1147,19 @@
         <v>16</v>
       </c>
       <c r="D17" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F17" t="s">
         <v>15</v>
       </c>
       <c r="G17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I17">
         <v>2.5656560000000002</v>
       </c>
       <c r="J17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
@@ -1173,19 +1173,19 @@
         <v>16</v>
       </c>
       <c r="D18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F18" t="s">
         <v>15</v>
       </c>
       <c r="G18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I18">
         <v>7.6577999999999999</v>
       </c>
       <c r="J18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
@@ -1199,19 +1199,19 @@
         <v>16</v>
       </c>
       <c r="D19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F19" t="s">
         <v>15</v>
       </c>
       <c r="G19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I19">
         <v>6.5465999999999998</v>
       </c>
       <c r="J19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
@@ -1231,13 +1231,13 @@
         <v>15</v>
       </c>
       <c r="G20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I20">
         <v>5.5465999999999998</v>
       </c>
       <c r="J20" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
@@ -1251,19 +1251,19 @@
         <v>16</v>
       </c>
       <c r="D21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F21" t="s">
         <v>15</v>
       </c>
       <c r="G21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I21">
         <v>4.6546000000000003</v>
       </c>
       <c r="J21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
@@ -1274,22 +1274,22 @@
         <v>10</v>
       </c>
       <c r="C22" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F22" t="s">
         <v>15</v>
       </c>
       <c r="G22" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I22">
         <v>1.6577999999999999</v>
       </c>
       <c r="J22" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
@@ -1300,22 +1300,22 @@
         <v>10</v>
       </c>
       <c r="C23" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F23" t="s">
         <v>15</v>
       </c>
       <c r="G23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I23">
         <v>1.5466</v>
       </c>
       <c r="J23" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
@@ -1329,19 +1329,19 @@
         <v>14</v>
       </c>
       <c r="D24" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F24" t="s">
         <v>15</v>
       </c>
       <c r="G24" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I24">
         <v>6.54</v>
       </c>
       <c r="J24" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
@@ -1352,22 +1352,22 @@
         <v>10</v>
       </c>
       <c r="C25" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D25" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F25" t="s">
         <v>15</v>
       </c>
       <c r="G25" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I25">
         <v>2</v>
       </c>
       <c r="J25" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
@@ -1378,22 +1378,22 @@
         <v>10</v>
       </c>
       <c r="C26" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F26" t="s">
         <v>15</v>
       </c>
       <c r="G26" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I26">
         <v>4.6546000000000003</v>
       </c>
       <c r="J26" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
@@ -1407,19 +1407,19 @@
         <v>16</v>
       </c>
       <c r="D27" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F27" t="s">
         <v>15</v>
       </c>
       <c r="G27" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I27">
         <v>3.4540000000000002</v>
       </c>
       <c r="J27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1464,7 +1464,7 @@
         <v>12</v>
       </c>
       <c r="E1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F1" t="s">
         <v>13</v>
@@ -1493,19 +1493,19 @@
         <v>14</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F2" t="s">
         <v>15</v>
       </c>
       <c r="G2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I2">
         <v>4.6546000000000003</v>
       </c>
       <c r="J2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -1516,22 +1516,22 @@
         <v>10</v>
       </c>
       <c r="C3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D3" t="s">
         <v>62</v>
       </c>
-      <c r="D3" t="s">
-        <v>63</v>
-      </c>
       <c r="F3" t="s">
         <v>15</v>
       </c>
       <c r="G3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I3">
         <v>2</v>
       </c>
       <c r="J3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
@@ -1557,7 +1557,7 @@
         <v>1.2465999999999999</v>
       </c>
       <c r="J4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
@@ -1571,19 +1571,19 @@
         <v>16</v>
       </c>
       <c r="D5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F5" t="s">
         <v>15</v>
       </c>
       <c r="G5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I5">
         <v>2.5656560000000002</v>
       </c>
       <c r="J5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
@@ -1597,19 +1597,19 @@
         <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F6" t="s">
         <v>15</v>
       </c>
       <c r="G6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I6">
         <v>7.6577999999999999</v>
       </c>
       <c r="J6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
@@ -1623,19 +1623,19 @@
         <v>16</v>
       </c>
       <c r="D7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F7" t="s">
         <v>15</v>
       </c>
       <c r="G7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I7">
         <v>6.5465999999999998</v>
       </c>
       <c r="J7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
@@ -1655,13 +1655,13 @@
         <v>15</v>
       </c>
       <c r="G8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I8">
         <v>5.5465999999999998</v>
       </c>
       <c r="J8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
@@ -1675,19 +1675,19 @@
         <v>16</v>
       </c>
       <c r="D9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F9" t="s">
         <v>15</v>
       </c>
       <c r="G9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I9">
         <v>4.6546000000000003</v>
       </c>
       <c r="J9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
@@ -1698,22 +1698,22 @@
         <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F10" t="s">
         <v>15</v>
       </c>
       <c r="G10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I10">
         <v>1.6577999999999999</v>
       </c>
       <c r="J10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
@@ -1724,22 +1724,22 @@
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F11" t="s">
         <v>15</v>
       </c>
       <c r="G11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I11">
         <v>1.5466</v>
       </c>
       <c r="J11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
@@ -1753,19 +1753,19 @@
         <v>14</v>
       </c>
       <c r="D12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F12" t="s">
         <v>15</v>
       </c>
       <c r="G12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I12">
         <v>6.54</v>
       </c>
       <c r="J12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
@@ -1776,22 +1776,22 @@
         <v>10</v>
       </c>
       <c r="C13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F13" t="s">
         <v>15</v>
       </c>
       <c r="G13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I13">
         <v>2</v>
       </c>
       <c r="J13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
@@ -1802,22 +1802,22 @@
         <v>10</v>
       </c>
       <c r="C14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F14" t="s">
         <v>15</v>
       </c>
       <c r="G14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I14">
         <v>4.6546000000000003</v>
       </c>
       <c r="J14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
@@ -1831,19 +1831,19 @@
         <v>16</v>
       </c>
       <c r="D15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F15" t="s">
         <v>15</v>
       </c>
       <c r="G15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I15">
         <v>3.4540000000000002</v>
       </c>
       <c r="J15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1855,8 +1855,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DF9FD88-E986-47BB-BEBA-C46BCE6B1675}">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1887,7 +1887,7 @@
         <v>12</v>
       </c>
       <c r="E1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F1" t="s">
         <v>13</v>
@@ -1922,7 +1922,7 @@
         <v>15</v>
       </c>
       <c r="G2" t="s">
-        <v>19</v>
+        <v>73</v>
       </c>
       <c r="H2" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
Inventory Transactions Location Add Location TO Location
</commit_message>
<xml_diff>
--- a/templates/LocationToLocation.xlsx
+++ b/templates/LocationToLocation.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\provar\rsqasampleproj\rsqasampleproj\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADA8EB60-665C-4675-83DE-9DF5C995C2AD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{035D0A60-3B1D-4A57-80DE-A9E452269690}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{AAD229B4-EC82-43D3-8B6F-DC67705348E6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="73">
   <si>
     <t>Item Name</t>
   </si>
@@ -63,9 +63,6 @@
   </si>
   <si>
     <t>Quantity To Transfer</t>
-  </si>
-  <si>
-    <t>P0303</t>
   </si>
   <si>
     <t>MS-Lot track item (Lot track item)</t>
@@ -653,13 +650,13 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" t="s">
         <v>12</v>
-      </c>
-      <c r="E1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F1" t="s">
-        <v>13</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>6</v>
@@ -671,7 +668,7 @@
         <v>8</v>
       </c>
       <c r="J1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
@@ -679,31 +676,31 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D2">
         <v>777</v>
       </c>
       <c r="E2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I2">
         <v>15</v>
       </c>
       <c r="J2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -711,31 +708,31 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D3">
         <v>777</v>
       </c>
       <c r="E3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" t="s">
         <v>24</v>
       </c>
-      <c r="F3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" t="s">
-        <v>25</v>
-      </c>
       <c r="H3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I3">
         <v>5</v>
       </c>
       <c r="J3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
@@ -743,31 +740,31 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D4">
         <v>777</v>
       </c>
       <c r="E4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" t="s">
         <v>27</v>
-      </c>
-      <c r="H4" t="s">
-        <v>28</v>
       </c>
       <c r="I4">
         <v>6</v>
       </c>
       <c r="J4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
@@ -775,31 +772,31 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D5">
         <v>777</v>
       </c>
       <c r="E5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H5" t="s">
         <v>30</v>
-      </c>
-      <c r="H5" t="s">
-        <v>31</v>
       </c>
       <c r="I5">
         <v>8</v>
       </c>
       <c r="J5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
@@ -807,31 +804,31 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D6">
         <v>777</v>
       </c>
       <c r="E6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G6" t="s">
+        <v>37</v>
+      </c>
+      <c r="H6" t="s">
         <v>38</v>
-      </c>
-      <c r="H6" t="s">
-        <v>39</v>
       </c>
       <c r="I6">
         <v>75</v>
       </c>
       <c r="J6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
@@ -839,31 +836,31 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G7" t="s">
+        <v>37</v>
+      </c>
+      <c r="H7" t="s">
         <v>38</v>
-      </c>
-      <c r="H7" t="s">
-        <v>39</v>
       </c>
       <c r="I7">
         <v>5</v>
       </c>
       <c r="J7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
@@ -871,31 +868,31 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H8" t="s">
         <v>30</v>
-      </c>
-      <c r="H8" t="s">
-        <v>31</v>
       </c>
       <c r="I8">
         <v>4.5490000000000004</v>
       </c>
       <c r="J8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
@@ -903,31 +900,31 @@
         <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" t="s">
+        <v>19</v>
+      </c>
+      <c r="H9" t="s">
         <v>28</v>
-      </c>
-      <c r="E9" t="s">
-        <v>24</v>
-      </c>
-      <c r="F9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G9" t="s">
-        <v>20</v>
-      </c>
-      <c r="H9" t="s">
-        <v>29</v>
       </c>
       <c r="I9">
         <v>3.3544999999999998</v>
       </c>
       <c r="J9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
@@ -935,31 +932,31 @@
         <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F10">
         <v>1003</v>
       </c>
       <c r="G10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I10">
         <v>11.656478999999999</v>
       </c>
       <c r="J10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
@@ -967,31 +964,31 @@
         <v>4</v>
       </c>
       <c r="B11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D11" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" t="s">
+        <v>43</v>
+      </c>
+      <c r="F11" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11" t="s">
         <v>41</v>
       </c>
-      <c r="E11" t="s">
-        <v>44</v>
-      </c>
-      <c r="F11" t="s">
-        <v>15</v>
-      </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
         <v>42</v>
-      </c>
-      <c r="H11" t="s">
-        <v>43</v>
       </c>
       <c r="I11">
         <v>2.6558999999999999</v>
       </c>
       <c r="J11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
@@ -999,63 +996,63 @@
         <v>4</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D12" t="s">
+        <v>44</v>
+      </c>
+      <c r="E12" t="s">
         <v>45</v>
-      </c>
-      <c r="E12" t="s">
-        <v>46</v>
       </c>
       <c r="F12">
         <v>1005</v>
       </c>
       <c r="G12" t="s">
+        <v>37</v>
+      </c>
+      <c r="H12" t="s">
         <v>38</v>
-      </c>
-      <c r="H12" t="s">
-        <v>39</v>
       </c>
       <c r="I12">
         <v>30.545999999999999</v>
       </c>
       <c r="J12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D13">
         <v>1</v>
       </c>
       <c r="E13" t="s">
+        <v>35</v>
+      </c>
+      <c r="F13" t="s">
+        <v>14</v>
+      </c>
+      <c r="G13" t="s">
+        <v>22</v>
+      </c>
+      <c r="H13" t="s">
         <v>36</v>
-      </c>
-      <c r="F13" t="s">
-        <v>15</v>
-      </c>
-      <c r="G13" t="s">
-        <v>23</v>
-      </c>
-      <c r="H13" t="s">
-        <v>37</v>
       </c>
       <c r="I13">
         <v>1</v>
       </c>
       <c r="J13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
@@ -1063,25 +1060,25 @@
         <v>4</v>
       </c>
       <c r="B14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I14">
         <v>4.6546000000000003</v>
       </c>
       <c r="J14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
@@ -1089,25 +1086,25 @@
         <v>4</v>
       </c>
       <c r="B15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C15" t="s">
+        <v>60</v>
+      </c>
+      <c r="D15" t="s">
         <v>61</v>
       </c>
-      <c r="D15" t="s">
-        <v>62</v>
-      </c>
       <c r="F15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I15">
         <v>2</v>
       </c>
       <c r="J15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
@@ -1115,25 +1112,25 @@
         <v>4</v>
       </c>
       <c r="B16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D16">
         <v>1906</v>
       </c>
       <c r="F16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I16">
         <v>1.2465999999999999</v>
       </c>
       <c r="J16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
@@ -1141,25 +1138,25 @@
         <v>4</v>
       </c>
       <c r="B17" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D17" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I17">
         <v>2.5656560000000002</v>
       </c>
       <c r="J17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
@@ -1167,25 +1164,25 @@
         <v>4</v>
       </c>
       <c r="B18" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I18">
         <v>7.6577999999999999</v>
       </c>
       <c r="J18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
@@ -1193,25 +1190,25 @@
         <v>4</v>
       </c>
       <c r="B19" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D19" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I19">
         <v>6.5465999999999998</v>
       </c>
       <c r="J19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
@@ -1219,25 +1216,25 @@
         <v>4</v>
       </c>
       <c r="B20" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D20">
         <v>1906</v>
       </c>
       <c r="F20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I20">
         <v>5.5465999999999998</v>
       </c>
       <c r="J20" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
@@ -1245,25 +1242,25 @@
         <v>4</v>
       </c>
       <c r="B21" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C21" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I21">
         <v>4.6546000000000003</v>
       </c>
       <c r="J21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
@@ -1271,25 +1268,25 @@
         <v>4</v>
       </c>
       <c r="B22" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G22" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I22">
         <v>1.6577999999999999</v>
       </c>
       <c r="J22" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
@@ -1297,25 +1294,25 @@
         <v>4</v>
       </c>
       <c r="B23" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C23" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F23" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G23" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I23">
         <v>1.5466</v>
       </c>
       <c r="J23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
@@ -1323,25 +1320,25 @@
         <v>4</v>
       </c>
       <c r="B24" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C24" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D24" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G24" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I24">
         <v>6.54</v>
       </c>
       <c r="J24" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
@@ -1349,25 +1346,25 @@
         <v>4</v>
       </c>
       <c r="B25" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C25" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D25" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F25" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G25" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I25">
         <v>2</v>
       </c>
       <c r="J25" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
@@ -1375,25 +1372,25 @@
         <v>4</v>
       </c>
       <c r="B26" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C26" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F26" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G26" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I26">
         <v>4.6546000000000003</v>
       </c>
       <c r="J26" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
@@ -1401,25 +1398,25 @@
         <v>4</v>
       </c>
       <c r="B27" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C27" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D27" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F27" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G27" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I27">
         <v>3.4540000000000002</v>
       </c>
       <c r="J27" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1461,13 +1458,13 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" t="s">
         <v>12</v>
-      </c>
-      <c r="E1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F1" t="s">
-        <v>13</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>6</v>
@@ -1479,7 +1476,7 @@
         <v>8</v>
       </c>
       <c r="J1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
@@ -1487,25 +1484,25 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I2">
         <v>4.6546000000000003</v>
       </c>
       <c r="J2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -1513,25 +1510,25 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D3" t="s">
         <v>61</v>
       </c>
-      <c r="D3" t="s">
-        <v>62</v>
-      </c>
       <c r="F3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I3">
         <v>2</v>
       </c>
       <c r="J3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
@@ -1539,25 +1536,25 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D4">
         <v>1906</v>
       </c>
       <c r="F4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I4">
         <v>1.2465999999999999</v>
       </c>
       <c r="J4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
@@ -1565,25 +1562,25 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I5">
         <v>2.5656560000000002</v>
       </c>
       <c r="J5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
@@ -1591,25 +1588,25 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I6">
         <v>7.6577999999999999</v>
       </c>
       <c r="J6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
@@ -1617,25 +1614,25 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I7">
         <v>6.5465999999999998</v>
       </c>
       <c r="J7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
@@ -1643,25 +1640,25 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D8">
         <v>1906</v>
       </c>
       <c r="F8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I8">
         <v>5.5465999999999998</v>
       </c>
       <c r="J8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
@@ -1669,25 +1666,25 @@
         <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I9">
         <v>4.6546000000000003</v>
       </c>
       <c r="J9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
@@ -1695,25 +1692,25 @@
         <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I10">
         <v>1.6577999999999999</v>
       </c>
       <c r="J10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
@@ -1721,25 +1718,25 @@
         <v>4</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I11">
         <v>1.5466</v>
       </c>
       <c r="J11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
@@ -1747,25 +1744,25 @@
         <v>4</v>
       </c>
       <c r="B12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I12">
         <v>6.54</v>
       </c>
       <c r="J12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
@@ -1773,25 +1770,25 @@
         <v>4</v>
       </c>
       <c r="B13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I13">
         <v>2</v>
       </c>
       <c r="J13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
@@ -1799,25 +1796,25 @@
         <v>4</v>
       </c>
       <c r="B14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I14">
         <v>4.6546000000000003</v>
       </c>
       <c r="J14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
@@ -1825,25 +1822,25 @@
         <v>4</v>
       </c>
       <c r="B15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I15">
         <v>3.4540000000000002</v>
       </c>
       <c r="J15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1856,7 +1853,7 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1884,13 +1881,13 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" t="s">
         <v>12</v>
-      </c>
-      <c r="E1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F1" t="s">
-        <v>13</v>
       </c>
       <c r="G1" t="s">
         <v>3</v>
@@ -1902,7 +1899,7 @@
         <v>7</v>
       </c>
       <c r="J1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
@@ -1913,25 +1910,22 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D2">
         <v>2007</v>
       </c>
       <c r="F2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" t="s">
         <v>17</v>
-      </c>
-      <c r="I2" t="s">
-        <v>9</v>
-      </c>
-      <c r="J2" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Code For RSTK-8173 Modification related to connection name and variables
</commit_message>
<xml_diff>
--- a/templates/LocationToLocation.xlsx
+++ b/templates/LocationToLocation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\provar\rsqasampleproj\rsqasampleproj\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{035D0A60-3B1D-4A57-80DE-A9E452269690}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2E5E708-C5FC-44C5-895E-D52AF7C16268}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{AAD229B4-EC82-43D3-8B6F-DC67705348E6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="74">
   <si>
     <t>Item Name</t>
   </si>
@@ -254,7 +254,10 @@
     <t>P-5V1I</t>
   </si>
   <si>
-    <t>Provar-120,Provar-121</t>
+    <t>P-CUF3</t>
+  </si>
+  <si>
+    <t>Provar-169,Provar-170,Provar-171</t>
   </si>
 </sst>
 </file>
@@ -624,7 +627,7 @@
   <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1853,7 +1856,7 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1919,16 +1922,20 @@
         <v>14</v>
       </c>
       <c r="G2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H2" t="s">
         <v>16</v>
       </c>
+      <c r="I2" t="s">
+        <v>72</v>
+      </c>
       <c r="J2" t="s">
         <v>17</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>